<commit_message>
Adição das planilhas das falhas: FSeQ, FADG e FADO.
</commit_message>
<xml_diff>
--- a/planilhas/deteccao/FSeDG/melhores.xlsx
+++ b/planilhas/deteccao/FSeDG/melhores.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="EstaPasta_de_trabalho" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="195" windowWidth="19320" windowHeight="12015"/>
@@ -14,12 +14,12 @@
     <externalReference r:id="rId3"/>
     <externalReference r:id="rId4"/>
   </externalReferences>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
   <si>
     <t>Treinamento</t>
   </si>
@@ -52,37 +52,13 @@
   </si>
   <si>
     <t>Obs.: Este arquivo faz referência aos outros arquivos da pasta, portanto não pode ser movido para outro local.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Valor do ganho do sensor variando em </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>±</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 20%</t>
-    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,12 +104,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -189,7 +159,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -226,9 +196,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -246,7 +213,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="N8"/>
@@ -261,22 +228,22 @@
       <sheetData sheetId="3">
         <row r="11">
           <cell r="B11">
-            <v>12</v>
+            <v>16</v>
           </cell>
           <cell r="C11">
-            <v>4</v>
+            <v>1</v>
           </cell>
           <cell r="D11">
-            <v>23460</v>
+            <v>23430</v>
           </cell>
           <cell r="E11">
-            <v>196.33333333333334</v>
+            <v>133.66666666666666</v>
           </cell>
           <cell r="F11">
-            <v>343.66666666666669</v>
+            <v>436.33333333333331</v>
           </cell>
           <cell r="G11">
-            <v>540</v>
+            <v>570</v>
           </cell>
         </row>
       </sheetData>
@@ -286,7 +253,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="N14"/>
@@ -301,22 +268,22 @@
       <sheetData sheetId="3">
         <row r="11">
           <cell r="B11">
-            <v>18</v>
+            <v>22</v>
           </cell>
           <cell r="C11">
-            <v>2</v>
+            <v>6</v>
           </cell>
           <cell r="D11">
-            <v>23455</v>
+            <v>23456.333333333332</v>
           </cell>
           <cell r="E11">
-            <v>300.33333333333331</v>
+            <v>176</v>
           </cell>
           <cell r="F11">
-            <v>244.66666666666666</v>
+            <v>367.66666666666669</v>
           </cell>
           <cell r="G11">
-            <v>545</v>
+            <v>543.66666666666674</v>
           </cell>
         </row>
       </sheetData>
@@ -326,7 +293,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="N20"/>
@@ -341,22 +308,22 @@
       <sheetData sheetId="3">
         <row r="11">
           <cell r="B11">
-            <v>20</v>
+            <v>28</v>
           </cell>
           <cell r="C11">
             <v>2</v>
           </cell>
           <cell r="D11">
-            <v>23518.666666666668</v>
+            <v>23491.333333333332</v>
           </cell>
           <cell r="E11">
-            <v>160.33333333333334</v>
+            <v>203.33333333333334</v>
           </cell>
           <cell r="F11">
-            <v>321</v>
+            <v>305.33333333333331</v>
           </cell>
           <cell r="G11">
-            <v>481.33333333333337</v>
+            <v>508.66666666666663</v>
           </cell>
         </row>
       </sheetData>
@@ -440,7 +407,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -475,7 +441,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Escritório">
@@ -651,15 +616,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Plan4"/>
-  <dimension ref="B2:J13"/>
+  <dimension ref="B2:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="1.42578125" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" customWidth="1"/>
@@ -669,238 +634,226 @@
     <col min="9" max="9" width="1.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
+    <row r="2" spans="2:10">
+      <c r="B2" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
+    <row r="4" spans="2:10" ht="15" customHeight="1">
+      <c r="B4" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
     </row>
-    <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="11" t="s">
+    <row r="5" spans="2:10">
+      <c r="B5" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10">
+      <c r="B6" s="5">
+        <v>2</v>
+      </c>
+      <c r="C6" s="10">
+        <f>[1]Melhores!B$11</f>
+        <v>16</v>
+      </c>
+      <c r="D6" s="10">
+        <f>[1]Melhores!C$11</f>
         <v>1</v>
       </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
+      <c r="E6" s="10">
+        <f>[1]Melhores!D$11</f>
+        <v>23430</v>
+      </c>
+      <c r="F6" s="10">
+        <f>[1]Melhores!E$11</f>
+        <v>133.66666666666666</v>
+      </c>
+      <c r="G6" s="10">
+        <f>[1]Melhores!F$11</f>
+        <v>436.33333333333331</v>
+      </c>
+      <c r="H6" s="10">
+        <f>[1]Melhores!G$11</f>
+        <v>570</v>
+      </c>
+      <c r="J6" s="4" t="str">
+        <f ca="1">IF(H6=MIN($H$6:$H$8),CELL("lin",H6),"")</f>
+        <v/>
+      </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E6" s="8" t="s">
+    <row r="7" spans="2:10">
+      <c r="B7" s="5">
+        <v>3</v>
+      </c>
+      <c r="C7" s="10">
+        <f>[2]Melhores!B$11</f>
+        <v>22</v>
+      </c>
+      <c r="D7" s="10">
+        <f>[2]Melhores!C$11</f>
+        <v>6</v>
+      </c>
+      <c r="E7" s="10">
+        <f>[2]Melhores!D$11</f>
+        <v>23456.333333333332</v>
+      </c>
+      <c r="F7" s="10">
+        <f>[2]Melhores!E$11</f>
+        <v>176</v>
+      </c>
+      <c r="G7" s="10">
+        <f>[2]Melhores!F$11</f>
+        <v>367.66666666666669</v>
+      </c>
+      <c r="H7" s="10">
+        <f>[2]Melhores!G$11</f>
+        <v>543.66666666666674</v>
+      </c>
+      <c r="J7" s="4" t="str">
+        <f t="shared" ref="J7:J8" ca="1" si="0">IF(H7=MIN($H$6:$H$8),CELL("lin",H7),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="2:10">
+      <c r="B8" s="5">
         <v>4</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="5">
-        <v>2</v>
-      </c>
-      <c r="C7" s="10">
-        <f>[1]Melhores!B$11</f>
-        <v>12</v>
-      </c>
-      <c r="D7" s="10">
-        <f>[1]Melhores!C$11</f>
-        <v>4</v>
-      </c>
-      <c r="E7" s="10">
-        <f>[1]Melhores!D$11</f>
-        <v>23460</v>
-      </c>
-      <c r="F7" s="10">
-        <f>[1]Melhores!E$11</f>
-        <v>196.33333333333334</v>
-      </c>
-      <c r="G7" s="10">
-        <f>[1]Melhores!F$11</f>
-        <v>343.66666666666669</v>
-      </c>
-      <c r="H7" s="10">
-        <f>[1]Melhores!G$11</f>
-        <v>540</v>
-      </c>
-      <c r="J7" s="4" t="str">
-        <f ca="1">IF(H7=MIN($H$7:$H$9),CELL("lin",H7),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="5">
-        <v>3</v>
-      </c>
       <c r="C8" s="10">
-        <f>[2]Melhores!B$11</f>
-        <v>18</v>
+        <f>[3]Melhores!B$11</f>
+        <v>28</v>
       </c>
       <c r="D8" s="10">
-        <f>[2]Melhores!C$11</f>
-        <v>2</v>
-      </c>
-      <c r="E8" s="10">
-        <f>[2]Melhores!D$11</f>
-        <v>23455</v>
-      </c>
-      <c r="F8" s="10">
-        <f>[2]Melhores!E$11</f>
-        <v>300.33333333333331</v>
-      </c>
-      <c r="G8" s="10">
-        <f>[2]Melhores!F$11</f>
-        <v>244.66666666666666</v>
-      </c>
-      <c r="H8" s="10">
-        <f>[2]Melhores!G$11</f>
-        <v>545</v>
-      </c>
-      <c r="J8" s="4" t="str">
-        <f t="shared" ref="J8:J9" ca="1" si="0">IF(H8=MIN($H$7:$H$9),CELL("lin",H8),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="5">
-        <v>4</v>
-      </c>
-      <c r="C9" s="10">
-        <f>[3]Melhores!B$11</f>
-        <v>20</v>
-      </c>
-      <c r="D9" s="10">
         <f>[3]Melhores!C$11</f>
         <v>2</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E8" s="10">
         <f>[3]Melhores!D$11</f>
-        <v>23518.666666666668</v>
-      </c>
-      <c r="F9" s="10">
+        <v>23491.333333333332</v>
+      </c>
+      <c r="F8" s="10">
         <f>[3]Melhores!E$11</f>
-        <v>160.33333333333334</v>
-      </c>
-      <c r="G9" s="10">
+        <v>203.33333333333334</v>
+      </c>
+      <c r="G8" s="10">
         <f>[3]Melhores!F$11</f>
-        <v>321</v>
-      </c>
-      <c r="H9" s="10">
+        <v>305.33333333333331</v>
+      </c>
+      <c r="H8" s="10">
         <f>[3]Melhores!G$11</f>
-        <v>481.33333333333337</v>
-      </c>
-      <c r="J9" s="4">
+        <v>508.66666666666663</v>
+      </c>
+      <c r="J8" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="12" t="s">
+    <row r="10" spans="2:10">
+      <c r="B10" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="7" t="s">
+    <row r="11" spans="2:10">
+      <c r="B11" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C11" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D11" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E11" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="F11" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="G11" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H12" s="7" t="s">
+      <c r="H11" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="3">
-        <f ca="1">INDIRECT(CONCATENATE("$B$",SUM($J$7:$J$9)))</f>
+    <row r="12" spans="2:10">
+      <c r="B12" s="3">
+        <f ca="1">INDIRECT(CONCATENATE("$B$",SUM($J$6:$J$8)))</f>
         <v>4</v>
       </c>
-      <c r="C13" s="3">
-        <f ca="1">INDIRECT(CONCATENATE("$C$",SUM($J$7:$J$9)))</f>
-        <v>20</v>
-      </c>
-      <c r="D13" s="3">
-        <f ca="1">INDIRECT(CONCATENATE("$D$",SUM($J$7:$J$9)))</f>
+      <c r="C12" s="3">
+        <f ca="1">INDIRECT(CONCATENATE("$C$",SUM($J$6:$J$8)))</f>
+        <v>28</v>
+      </c>
+      <c r="D12" s="3">
+        <f ca="1">INDIRECT(CONCATENATE("$D$",SUM($J$6:$J$8)))</f>
         <v>2</v>
       </c>
-      <c r="E13" s="3">
-        <f ca="1">INDIRECT(CONCATENATE("$E$",SUM($J$7:$J$9)))</f>
-        <v>23518.666666666668</v>
-      </c>
-      <c r="F13" s="3">
-        <f ca="1">INDIRECT(CONCATENATE("$F$",SUM($J$7:$J$9)))</f>
-        <v>160.33333333333334</v>
-      </c>
-      <c r="G13" s="3">
-        <f ca="1">INDIRECT(CONCATENATE("$G$",SUM($J$7:$J$9)))</f>
-        <v>321</v>
-      </c>
-      <c r="H13" s="3">
-        <f ca="1">INDIRECT(CONCATENATE("$H$",SUM($J$7:$J$9)))</f>
-        <v>481.33333333333337</v>
+      <c r="E12" s="3">
+        <f ca="1">INDIRECT(CONCATENATE("$E$",SUM($J$6:$J$8)))</f>
+        <v>23491.333333333332</v>
+      </c>
+      <c r="F12" s="3">
+        <f ca="1">INDIRECT(CONCATENATE("$F$",SUM($J$6:$J$8)))</f>
+        <v>203.33333333333334</v>
+      </c>
+      <c r="G12" s="3">
+        <f ca="1">INDIRECT(CONCATENATE("$G$",SUM($J$6:$J$8)))</f>
+        <v>305.33333333333331</v>
+      </c>
+      <c r="H12" s="3">
+        <f ca="1">INDIRECT(CONCATENATE("$H$",SUM($J$6:$J$8)))</f>
+        <v>508.66666666666663</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B5:H5"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="B3:H3"/>
+  <mergeCells count="3">
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="B10:H10"/>
     <mergeCell ref="B2:H2"/>
   </mergeCells>
-  <conditionalFormatting sqref="H7:H9">
+  <conditionalFormatting sqref="H6:H8">
     <cfRule type="colorScale" priority="1">
       <colorScale>
-        <cfvo type="min"/>
+        <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>

</xml_diff>